<commit_message>
Testing implemented. Excel File updated with TRUE or FALSE if action completed succesfully for create, read, update, and delete.
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\Repos\CMPG-323-Project-4---35314389\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DE4E73-674E-4D4D-87C3-8DF5E98515BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4164" yWindow="3048" windowWidth="17280" windowHeight="8772" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -280,16 +280,16 @@
     <t>C05</t>
   </si>
   <si>
+    <t>Read Test Passed</t>
+  </si>
+  <si>
+    <t>Update Test Passed</t>
+  </si>
+  <si>
+    <t>Delete Test Passed</t>
+  </si>
+  <si>
     <t>Create Test Passed</t>
-  </si>
-  <si>
-    <t>Read Test Passed</t>
-  </si>
-  <si>
-    <t>Update Test Passed</t>
-  </si>
-  <si>
-    <t>Delete Test Passed</t>
   </si>
 </sst>
 </file>
@@ -690,16 +690,16 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -719,7 +719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
@@ -739,7 +739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>50</v>
       </c>
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -799,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>52</v>
       </c>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -859,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>55</v>
       </c>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
@@ -914,13 +914,13 @@
       <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -931,7 +931,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -942,7 +942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -953,7 +953,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -964,7 +964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -975,7 +975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -986,7 +986,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -997,7 +997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
@@ -1044,14 +1044,14 @@
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
@@ -1127,424 +1127,424 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>